<commit_message>
Added more hand-verified sequence sheets
</commit_message>
<xml_diff>
--- a/backend/evaluation/evaluation_sheets/83.xlsx
+++ b/backend/evaluation/evaluation_sheets/83.xlsx
@@ -5,26 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianruhle/Studium/Master/FSS24/Project/lasso-python/backend/evaluation/evaluation_sheets/llm_sequence_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Desktop/flo projekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AAFD6D-F116-B747-9A74-E683801602D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226337E5-5859-424F-BAA3-318C0277BACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="740" windowWidth="15000" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>create</t>
   </si>
   <si>
+    <t>A1</t>
+  </si>
+  <si>
     <t>Task83</t>
   </si>
   <si>
@@ -34,16 +37,16 @@
     <t>f</t>
   </si>
   <si>
+    <t>abc</t>
+  </si>
+  <si>
     <t>t</t>
   </si>
   <si>
+    <t>gfg</t>
+  </si>
+  <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>gfg</t>
   </si>
   <si>
     <t>ab</t>
@@ -86,7 +89,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="215" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -399,26 +402,32 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="C2" t="s">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -426,13 +435,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>